<commit_message>
添加测试表，完善 TableManager 功能 和 TableManagereExample 测试文件
</commit_message>
<xml_diff>
--- a/DataTables/Datas/__tables__.xlsx
+++ b/DataTables/Datas/__tables__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\LubanTest\Luban\MiniTemplate\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\GameFramework\DataTables\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FA6223-63FA-40AB-A4BC-8CBD3FED1689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A41BF4-2F5C-4FE6-8CC8-AAF7F5763992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12135" yWindow="9645" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11490" yWindow="8220" windowWidth="19500" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>##var</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>reward.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>demo.TBItem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>demo.Item</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>item.xlsx</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -466,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -585,6 +597,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>